<commit_message>
# Processed and imported honduras ff2.0 and coralnet (2021-2023) data to mermaid
</commit_message>
<xml_diff>
--- a/data/processed/honduras/ff2.0/hon_ff2.0_habitat_sites_processed.xlsx
+++ b/data/processed/honduras/ff2.0/hon_ff2.0_habitat_sites_processed.xlsx
@@ -411,10 +411,10 @@
         </is>
       </c>
       <c r="C2">
-        <v>16</v>
+        <v>16.03</v>
       </c>
       <c r="D2">
-        <v>-85</v>
+        <v>-85.15000000000001</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -449,10 +449,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>16.03</v>
       </c>
       <c r="D3">
-        <v>-85</v>
+        <v>-85.15000000000001</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>16</v>
+        <v>16.03</v>
       </c>
       <c r="D4">
-        <v>-85</v>
+        <v>-85.15000000000001</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -867,10 +867,10 @@
         </is>
       </c>
       <c r="C14">
-        <v>16.39</v>
+        <v>16.33</v>
       </c>
       <c r="D14">
-        <v>-86.26000000000001</v>
+        <v>-86.59</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="C15">
-        <v>16.39</v>
+        <v>16.33</v>
       </c>
       <c r="D15">
-        <v>-86.26000000000001</v>
+        <v>-86.59</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -943,10 +943,10 @@
         </is>
       </c>
       <c r="C16">
-        <v>16.39</v>
+        <v>16.33</v>
       </c>
       <c r="D16">
-        <v>-86.26000000000001</v>
+        <v>-86.59</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -981,10 +981,10 @@
         </is>
       </c>
       <c r="C17">
-        <v>16.39</v>
+        <v>16.33</v>
       </c>
       <c r="D17">
-        <v>-86.26000000000001</v>
+        <v>-86.59</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1019,10 +1019,10 @@
         </is>
       </c>
       <c r="C18">
-        <v>16.39</v>
+        <v>16.33</v>
       </c>
       <c r="D18">
-        <v>-86.26000000000001</v>
+        <v>-86.59</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1171,10 +1171,10 @@
         </is>
       </c>
       <c r="C22">
-        <v>16.39</v>
+        <v>16.33</v>
       </c>
       <c r="D22">
-        <v>-86.26000000000001</v>
+        <v>-86.59</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>

</xml_diff>